<commit_message>
Modifications to sensors page
Minor modification to Motor controller and test harness.  Changes to
sensor page to provide larger canvas for drawing test harness events
</commit_message>
<xml_diff>
--- a/img/Map dog co-ords to SVG picture.xlsx
+++ b/img/Map dog co-ords to SVG picture.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
   <si>
     <t>Centre</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>In the new picture one SVG 1pt  =  1mm</t>
+  </si>
+  <si>
+    <t>'[{"sensorName":"l_ear","x": 1158,"y":890,"angle":999},{"sensorName":"r_ear","x": 1242,"y":890,"angle":999},{"sensorName":"left","x": 1120,"y":1343,"angle":180},{"sensorName":"bl_corner","x": 1152,"y":1411,"angle":225},{"sensorName":"tail","x": 1200,"y":1430,"angle":270},{"sensorName":"br_corner","x": 1248,"y":1411,"angle":315},{"sensorName":"right","x": 1280,"y":1343,"angle":0}]</t>
   </si>
 </sst>
 </file>
@@ -424,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -585,12 +588,10 @@
         <v>14</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="0"/>
         <v>1158</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="1"/>
-        <v>857</v>
+        <v>890</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
@@ -607,12 +608,10 @@
         <v>15</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="0"/>
         <v>1242</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="1"/>
-        <v>857</v>
+        <v>890</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
@@ -629,11 +628,10 @@
         <v>9</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="0"/>
-        <v>1105</v>
+        <v>1120</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H9:H15" si="2">1200-C11</f>
         <v>1343</v>
       </c>
     </row>
@@ -651,12 +649,11 @@
         <v>10</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G9:G15" si="3">1200-D12</f>
         <v>1152</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="1"/>
-        <v>1390</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
@@ -673,12 +670,11 @@
         <v>11</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1200</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="1"/>
-        <v>1473</v>
+        <v>1430</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
@@ -695,12 +691,11 @@
         <v>12</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1248</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="1"/>
-        <v>1390</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
@@ -717,25 +712,29 @@
         <v>13</v>
       </c>
       <c r="G15" s="1">
-        <f t="shared" si="0"/>
-        <v>1295</v>
+        <v>1280</v>
       </c>
       <c r="H15" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1343</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>18</v>
       </c>

</xml_diff>